<commit_message>
to suppoer us stock
</commit_message>
<xml_diff>
--- a/outputs/20250717/backtest_report.xlsx
+++ b/outputs/20250717/backtest_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,336 +463,315 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-12-08</t>
+          <t>2024-12-22</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3353617370922525</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1582250066706042</v>
+        <v>0.09841994491865877</v>
       </c>
       <c r="D2" t="n">
-        <v>1.83511913320208</v>
+        <v>1.388418552533649</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.3432, 'KLAC': 0.23536, 'CBOE': 0.08915, 'COR': 0.08168, 'PM': 0.05394}</t>
+          <t>{'2330.TW': 0.10046, '2449.TW': 0.08815, '6669.TW': 0.08016, '2474.TW': 0.07576, '3702.TW': 0.07042}</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-12-22</t>
+          <t>2025-01-05</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3353617370922519</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1602468681479722</v>
+        <v>0.1003019146413577</v>
       </c>
       <c r="D3" t="n">
-        <v>1.811965128854384</v>
+        <v>1.362367587428499</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.3386, 'KLAC': 0.24506, 'CBOE': 0.08732, 'COR': 0.07689, 'PM': 0.04834}</t>
+          <t>{'2330.TW': 0.09495, '2449.TW': 0.08113, '6669.TW': 0.08079, '3702.TW': 0.07896, '2474.TW': 0.07139}</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2025-01-19</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3353617370922525</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1556303155865892</v>
+        <v>0.1009193956496041</v>
       </c>
       <c r="D4" t="n">
-        <v>1.865714504258664</v>
+        <v>1.354031864586792</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.33582, 'KLAC': 0.24286, 'CBOE': 0.08766, 'COR': 0.07282, 'PM': 0.04815}</t>
+          <t>{'2330.TW': 0.10031, '6669.TW': 0.08423, '2449.TW': 0.08299, '3702.TW': 0.08122, '2474.TW': 0.06991}</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-01-19</t>
+          <t>2025-02-02</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3353617370922535</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1488452942055652</v>
+        <v>0.0994157972633072</v>
       </c>
       <c r="D5" t="n">
-        <v>1.950761954833754</v>
+        <v>1.374510703791743</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.29769, 'KLAC': 0.23696, 'CBOE': 0.08586, 'COR': 0.06509, 'GOOGL': 0.04289}</t>
+          <t>{'2330.TW': 0.09815, '2449.TW': 0.0841, '3702.TW': 0.08041, '6669.TW': 0.07918, '2474.TW': 0.06798}</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-02</t>
+          <t>2025-02-16</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3353617370922537</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C6" t="n">
-        <v>0.148946080150259</v>
+        <v>0.09756232121158734</v>
       </c>
       <c r="D6" t="n">
-        <v>1.949441951069356</v>
+        <v>1.400623476024637</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.29651, 'KLAC': 0.23832, 'CBOE': 0.07822, 'COR': 0.06024, 'GOOGL': 0.03703}</t>
+          <t>{'2330.TW': 0.10165, '2449.TW': 0.08159, '6669.TW': 0.07751, '3702.TW': 0.07528, '2474.TW': 0.06702}</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-02-16</t>
+          <t>2025-03-02</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.335361737092254</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1396894106496323</v>
+        <v>0.093869136025188</v>
       </c>
       <c r="D7" t="n">
-        <v>2.078623825112532</v>
+        <v>1.455729574710677</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.28176, 'KLAC': 0.24031, 'CBOE': 0.08188, 'COR': 0.06122, 'COP': 0.03108}</t>
+          <t>{'2330.TW': 0.09895, '2449.TW': 0.07856, '6669.TW': 0.07496, '3702.TW': 0.07415, '2474.TW': 0.06688}</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-03-16</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3353617370922539</v>
+        <v>0.1516480774644057</v>
       </c>
       <c r="C8" t="n">
-        <v>0.145245959774592</v>
+        <v>0.09249499340045338</v>
       </c>
       <c r="D8" t="n">
-        <v>1.999103710305388</v>
+        <v>1.477356475639642</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.28921, 'KLAC': 0.24704, 'CBOE': 0.07942, 'COR': 0.06051, 'PM': 0.03477}</t>
+          <t>{'2330.TW': 0.10076, '2449.TW': 0.07817, '6669.TW': 0.07403, '3702.TW': 0.07351, '2474.TW': 0.07133}</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-03-16</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3353617370922541</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1422392398460258</v>
+        <v>0.09185067239047918</v>
       </c>
       <c r="D9" t="n">
-        <v>2.041361704453505</v>
+        <v>1.487719947040583</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.28761, 'KLAC': 0.23576, 'CBOE': 0.08093, 'COR': 0.06919, 'ELV': 0.04989}</t>
+          <t>{'2330.TW': 0.11101, '2449.TW': 0.07501, '3702.TW': 0.07415, '6669.TW': 0.06942, '2474.TW': 0.06705}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3353617370922541</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1386990494475748</v>
+        <v>0.1743576838845118</v>
       </c>
       <c r="D10" t="n">
-        <v>2.093465948387804</v>
+        <v>0.7837227153975975</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.28437, 'KLAC': 0.23583, 'CBOE': 0.07919, 'COR': 0.07455, 'ELV': 0.0491}</t>
+          <t>{'2449.TW': 0.23143, '2330.TW': 0.157, '1504.TW': 0.14353, '2474.TW': 0.10503, '3702.TW': 0.09154}</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-27</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3353617370922547</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1966955441396957</v>
+        <v>0.1669854087581121</v>
       </c>
       <c r="D11" t="n">
-        <v>1.476198855252339</v>
+        <v>0.8183234599997186</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.35194, 'KLAC': 0.20673, 'COR': 0.1305, 'ELV': 0.08949, 'CBOE': 0.08639}</t>
+          <t>{'2449.TW': 0.21053, '1504.TW': 0.1449, '2330.TW': 0.14223, '2474.TW': 0.10221, '3017.TW': 0.09631}</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-04-27</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3353617370922549</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2058935549451246</v>
+        <v>0.1591811668596504</v>
       </c>
       <c r="D12" t="n">
-        <v>1.410251705885806</v>
+        <v>0.8584437478391388</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.30858, 'KLAC': 0.25257, 'COR': 0.12178, 'CBOE': 0.09765, 'ELV': 0.07962}</t>
+          <t>{'2449.TW': 0.20328, '1504.TW': 0.14811, '2330.TW': 0.11889, '3017.TW': 0.10258, '2474.TW': 0.10179}</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-05-11</t>
+          <t>2025-05-25</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3353617370922549</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2004675773098629</v>
+        <v>0.1526547830051917</v>
       </c>
       <c r="D13" t="n">
-        <v>1.448422438125456</v>
+        <v>0.8951444217752307</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.31557, 'KLAC': 0.24914, 'COR': 0.10565, 'CBOE': 0.08267, 'ELV': 0.07268}</t>
+          <t>{'2449.TW': 0.19341, '1504.TW': 0.14442, '2330.TW': 0.11183, '3017.TW': 0.10496, '2474.TW': 0.0909}</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-05-25</t>
+          <t>2025-06-08</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3353617370922549</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1953135797477063</v>
+        <v>0.1484084686107517</v>
       </c>
       <c r="D14" t="n">
-        <v>1.486643875286735</v>
+        <v>0.9207566033364883</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.2926, 'KLAC': 0.26564, 'COR': 0.10504, 'CBOE': 0.09376, 'MKTX': 0.05807}</t>
+          <t>{'2449.TW': 0.18149, '1504.TW': 0.14117, '3017.TW': 0.10014, '2330.TW': 0.09647, '3702.TW': 0.08495}</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-06-08</t>
+          <t>2025-06-22</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3353617370922548</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1865028996272632</v>
+        <v>0.1430413222794237</v>
       </c>
       <c r="D15" t="n">
-        <v>1.556875188924995</v>
+        <v>0.9553049097062372</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>{'LKQ': 0.27708, 'KLAC': 0.26923, 'COR': 0.09872, 'CBOE': 0.08445, 'MKTX': 0.06038}</t>
+          <t>{'2449.TW': 0.17217, '1504.TW': 0.13281, '2330.TW': 0.09756, '3017.TW': 0.09327, '3702.TW': 0.08708}</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-06-22</t>
+          <t>2025-07-06</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3353617370922536</v>
+        <v>0.1516480774644056</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1810238965894229</v>
+        <v>0.1399883199739695</v>
       </c>
       <c r="D16" t="n">
-        <v>1.603996723984006</v>
+        <v>0.9761391342493072</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>{'KLAC': 0.27325, 'LKQ': 0.27185, 'COR': 0.0983, 'CBOE': 0.08374, 'KR': 0.06198}</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2025-07-06</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.3353617370922526</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.1647544887005503</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1.762390447643584</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>{'KLAC': 0.26238, 'LKQ': 0.23609, 'COR': 0.09021, 'CBOE': 0.08055, 'KR': 0.06102}</t>
+          <t>{'2449.TW': 0.1534, '1504.TW': 0.12779, '3017.TW': 0.08636, '2330.TW': 0.07912, '3702.TW': 0.07708}</t>
         </is>
       </c>
     </row>

</xml_diff>